<commit_message>
finishing up monthly bvr samples up to may 2025 (and 1 surprise fcr sample)
</commit_message>
<xml_diff>
--- a/Summer2022-2025-DataAnalysis/RawData/Zoop_sample_counting_template_2022-2025.xlsx
+++ b/Summer2022-2025-DataAnalysis/RawData/Zoop_sample_counting_template_2022-2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherwander/Documents/VirginiaTech/research/zooplankton/Summer2022-2025-DataAnalysis/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1437338-0F38-B743-80D4-499A3C290F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBDB9C9-E55A-0149-A8EB-B8D2CFFF12B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{3D67C25D-D874-DE45-AEE3-7A59E1B23F3C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="30">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -93,21 +93,6 @@
     <t>Keratella</t>
   </si>
   <si>
-    <t>Cal naup</t>
-  </si>
-  <si>
-    <t>1 mL</t>
-  </si>
-  <si>
-    <t>Ceriodaphnia</t>
-  </si>
-  <si>
-    <t>Conochiloides</t>
-  </si>
-  <si>
-    <t>B23Sep24_9m</t>
-  </si>
-  <si>
     <t>Daphnia</t>
   </si>
   <si>
@@ -117,16 +102,28 @@
     <t>Polyarthra</t>
   </si>
   <si>
-    <t>Calanoida</t>
-  </si>
-  <si>
     <t>B. longirostris</t>
   </si>
   <si>
-    <t>Hexarthra</t>
+    <t>Cal naup</t>
   </si>
   <si>
-    <t>Conochilus</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Chydoridae</t>
+  </si>
+  <si>
+    <t>Gastropus</t>
+  </si>
+  <si>
+    <t>F07Apr25_9m</t>
+  </si>
+  <si>
+    <t>2 mL</t>
+  </si>
+  <si>
+    <t>Monostyla</t>
   </si>
 </sst>
 </file>
@@ -527,10 +524,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D676C963-F956-4A49-8829-4831A47E6094}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD1048574"/>
+  <dimension ref="A1:XFD1048573"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C1"/>
       <c r="G1" s="6"/>
@@ -557,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>45558</v>
+        <v>45754</v>
       </c>
       <c r="C2"/>
     </row>
@@ -566,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>45451</v>
+        <v>45821</v>
       </c>
       <c r="C3"/>
     </row>
@@ -576,7 +573,7 @@
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -610,13 +607,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7">
-        <v>7.8</v>
+        <v>6.8</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>14</v>
@@ -630,13 +627,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>14</v>
@@ -645,20 +642,20 @@
         <v>1000</v>
       </c>
       <c r="F8" s="3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9">
-        <v>1.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>14</v>
@@ -666,19 +663,21 @@
       <c r="E9" s="3">
         <v>1000</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>5.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>14</v>
@@ -686,19 +685,21 @@
       <c r="E10" s="3">
         <v>1000</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3">
+        <v>0.8</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11">
-        <v>4.9000000000000004</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>14</v>
@@ -706,19 +707,21 @@
       <c r="E11" s="3">
         <v>1000</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3">
+        <v>0.8</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>5.0999999999999996</v>
+        <v>1</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>14</v>
@@ -726,19 +729,21 @@
       <c r="E12" s="3">
         <v>1000</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>0.8</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>14</v>
@@ -746,19 +751,21 @@
       <c r="E13" s="3">
         <v>1000</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>14</v>
@@ -767,7 +774,7 @@
         <v>1000</v>
       </c>
       <c r="F14" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="6"/>
@@ -780,7 +787,7 @@
         <v>12</v>
       </c>
       <c r="C15">
-        <v>5.3</v>
+        <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>14</v>
@@ -788,19 +795,21 @@
       <c r="E15" s="3">
         <v>1000</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3">
+        <v>0.5</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16">
-        <v>5.6</v>
+        <v>2.4</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>14</v>
@@ -820,7 +829,7 @@
         <v>12</v>
       </c>
       <c r="C17">
-        <v>3.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>14</v>
@@ -828,19 +837,21 @@
       <c r="E17" s="3">
         <v>1000</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>19</v>
+      <c r="A18" t="s">
+        <v>20</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>14</v>
@@ -848,19 +859,21 @@
       <c r="E18" s="3">
         <v>1000</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3">
+        <v>0.5</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19">
-        <v>2.1</v>
+        <v>1</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>14</v>
@@ -868,19 +881,21 @@
       <c r="E19" s="3">
         <v>1000</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>1.3</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>14</v>
@@ -888,19 +903,21 @@
       <c r="E20" s="3">
         <v>1000</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
       <c r="G20" s="3"/>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>14</v>
@@ -908,19 +925,21 @@
       <c r="E21" s="3">
         <v>1000</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3">
+        <v>0.5</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>14</v>
@@ -928,19 +947,21 @@
       <c r="E22" s="3">
         <v>1000</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3">
+        <v>0.7</v>
+      </c>
       <c r="G22" s="3"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23">
-        <v>1.2</v>
+        <v>1.7</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>14</v>
@@ -948,24 +969,22 @@
       <c r="E23" s="3">
         <v>1000</v>
       </c>
-      <c r="F23" s="3">
-        <v>0.8</v>
-      </c>
+      <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
       <c r="C24">
-        <v>5.9</v>
+        <v>1.9</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E24" s="3">
         <v>1000</v>
@@ -976,58 +995,60 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E25" s="3">
         <v>1000</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G25" s="3"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E26" s="3">
         <v>1000</v>
       </c>
       <c r="F26" s="3">
-        <v>1.1000000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
       <c r="C27">
-        <v>5.2</v>
+        <v>2.1</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E27" s="3">
         <v>1000</v>
@@ -1038,16 +1059,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E28" s="3">
         <v>1000</v>
@@ -1058,16 +1079,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E29" s="3">
         <v>1000</v>
@@ -1084,32 +1105,30 @@
         <v>12</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2.1</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E30" s="3">
         <v>1000</v>
       </c>
-      <c r="F30" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
       </c>
       <c r="C31">
-        <v>5.5</v>
+        <v>1.8</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E31" s="3">
         <v>1000</v>
@@ -1120,53 +1139,57 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
       </c>
       <c r="C32">
-        <v>6.6</v>
+        <v>1</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E32" s="3">
         <v>1000</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G32" s="3"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E33" s="3">
         <v>1000</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3">
+        <v>0.8</v>
+      </c>
       <c r="G33" s="3"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>16</v>
@@ -1174,15 +1197,13 @@
       <c r="E34" s="3">
         <v>1000</v>
       </c>
-      <c r="F34" s="4">
-        <v>0.5</v>
-      </c>
+      <c r="F34" s="3"/>
       <c r="G34" s="4"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
@@ -1197,20 +1218,20 @@
         <v>1000</v>
       </c>
       <c r="F35" s="4">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
       </c>
       <c r="C36">
-        <v>5.4</v>
+        <v>2.5</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>16</v>
@@ -1222,15 +1243,15 @@
       <c r="G36" s="4"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
       <c r="C37">
-        <v>3.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>16</v>
@@ -1238,19 +1259,21 @@
       <c r="E37" s="3">
         <v>1000</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="4">
+        <v>0.7</v>
+      </c>
       <c r="G37" s="4"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
       </c>
       <c r="C38">
-        <v>5.6</v>
+        <v>2.1</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>16</v>
@@ -1259,18 +1282,18 @@
         <v>1000</v>
       </c>
       <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>16</v>
@@ -1278,19 +1301,21 @@
       <c r="E39" s="3">
         <v>1000</v>
       </c>
-      <c r="F39" s="4"/>
+      <c r="F39" s="4">
+        <v>0.6</v>
+      </c>
       <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
       </c>
       <c r="C40">
-        <v>3.9</v>
+        <v>1.9</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>16</v>
@@ -1298,19 +1323,19 @@
       <c r="E40" s="3">
         <v>1000</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
         <v>12</v>
       </c>
       <c r="C41">
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>16</v>
@@ -1318,19 +1343,20 @@
       <c r="E41" s="3">
         <v>1000</v>
       </c>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3">
+        <v>0.5</v>
+      </c>
       <c r="G41" s="3"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>16</v>
@@ -1338,19 +1364,17 @@
       <c r="E42" s="3">
         <v>1000</v>
       </c>
-      <c r="F42" s="3"/>
+      <c r="F42" s="3">
+        <v>0.8</v>
+      </c>
       <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43">
-        <v>1.5</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C43"/>
       <c r="D43" s="8" t="s">
         <v>16</v>
       </c>
@@ -1361,15 +1385,15 @@
       <c r="G43" s="3"/>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
       </c>
       <c r="C44">
-        <v>1.9</v>
+        <v>1</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>16</v>
@@ -1377,20 +1401,17 @@
       <c r="E44" s="3">
         <v>1000</v>
       </c>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G44" s="3"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45">
-        <v>2.2999999999999998</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C45"/>
       <c r="D45" s="8" t="s">
         <v>16</v>
       </c>
@@ -1401,16 +1422,11 @@
       <c r="G45" s="3"/>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46">
-        <v>1.5</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C46"/>
       <c r="D46" s="8" t="s">
         <v>16</v>
       </c>
@@ -1421,16 +1437,11 @@
       <c r="G46" s="3"/>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C47"/>
       <c r="D47" s="8" t="s">
         <v>16</v>
       </c>
@@ -1439,18 +1450,13 @@
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="6"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48">
-        <v>1.2</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C48"/>
       <c r="D48" s="8" t="s">
         <v>16</v>
       </c>
@@ -1460,8 +1466,9 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+      <c r="XFD48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>17</v>
       </c>
@@ -1469,7 +1476,7 @@
         <v>12</v>
       </c>
       <c r="C49">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>16</v>
@@ -1479,19 +1486,13 @@
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="4"/>
-      <c r="XFD49" s="6"/>
-    </row>
-    <row r="50" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B50" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50">
-        <v>5.9</v>
-      </c>
+      <c r="C50"/>
       <c r="D50" s="8" t="s">
         <v>16</v>
       </c>
@@ -1502,16 +1503,11 @@
       <c r="G50" s="3"/>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51">
-        <v>2.2999999999999998</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C51"/>
       <c r="D51" s="8" t="s">
         <v>16</v>
       </c>
@@ -1522,15 +1518,15 @@
       <c r="G51" s="3"/>
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>16</v>
@@ -1538,21 +1534,19 @@
       <c r="E52" s="3">
         <v>1000</v>
       </c>
-      <c r="F52" s="3">
-        <v>0.8</v>
-      </c>
+      <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="6"/>
-    </row>
-    <row r="53" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>16</v>
@@ -1560,15 +1554,13 @@
       <c r="E53" s="3">
         <v>1000</v>
       </c>
-      <c r="F53" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="F53" s="3"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -1586,37 +1578,30 @@
       <c r="G54" s="3"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55">
-        <v>1.3</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C55"/>
       <c r="D55" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E55" s="3">
         <v>1000</v>
       </c>
-      <c r="F55" s="3">
-        <v>1</v>
-      </c>
+      <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>2.1</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>16</v>
@@ -1624,21 +1609,19 @@
       <c r="E56" s="3">
         <v>1000</v>
       </c>
-      <c r="F56" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
       </c>
       <c r="C57">
-        <v>2.2999999999999998</v>
+        <v>1.8</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>16</v>
@@ -1650,60 +1633,55 @@
       <c r="G57" s="3"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" t="s">
-        <v>12</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C58"/>
       <c r="D58" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E58" s="3">
         <v>1000</v>
       </c>
-      <c r="F58" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
       </c>
       <c r="C59">
-        <v>7.1</v>
+        <v>1</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E59" s="3">
         <v>1000</v>
       </c>
-      <c r="F59" s="3"/>
+      <c r="F59" s="3">
+        <v>0.5</v>
+      </c>
       <c r="G59" s="3"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
       </c>
       <c r="C60">
-        <v>5.8</v>
+        <v>1.4</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E60" s="3">
         <v>1000</v>
@@ -1712,18 +1690,18 @@
       <c r="G60" s="3"/>
       <c r="H60" s="6"/>
     </row>
-    <row r="61" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
       </c>
       <c r="C61">
-        <v>6.4</v>
+        <v>1.7</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E61" s="3">
         <v>1000</v>
@@ -1732,60 +1710,55 @@
       <c r="G61" s="3"/>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
         <v>12</v>
       </c>
       <c r="C62">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E62" s="3">
         <v>1000</v>
       </c>
-      <c r="F62" s="3"/>
+      <c r="F62" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G62" s="3"/>
       <c r="H62" s="6"/>
     </row>
-    <row r="63" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
       </c>
       <c r="C63">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E63" s="3">
         <v>1000</v>
       </c>
-      <c r="F63" s="3">
-        <v>0.7</v>
-      </c>
+      <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="6"/>
     </row>
-    <row r="64" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B64" t="s">
-        <v>12</v>
-      </c>
-      <c r="C64">
-        <v>1.5</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C64"/>
       <c r="D64" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E64" s="3">
         <v>1000</v>
@@ -1796,16 +1769,11 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B65" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65">
-        <v>1.6</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C65"/>
       <c r="D65" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E65" s="3">
         <v>1000</v>
@@ -1816,16 +1784,11 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66">
-        <v>1.8</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C66"/>
       <c r="D66" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E66" s="3">
         <v>1000</v>
@@ -1836,16 +1799,11 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67">
-        <v>1.6</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C67"/>
       <c r="D67" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E67" s="3">
         <v>1000</v>
@@ -1853,19 +1811,20 @@
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B68" t="s">
         <v>12</v>
       </c>
       <c r="C68">
-        <v>5.0999999999999996</v>
+        <v>1.7</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E68" s="3">
         <v>1000</v>
@@ -1873,100 +1832,98 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
         <v>12</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E69" s="3">
         <v>1000</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
-      <c r="H69" s="6"/>
+      <c r="H69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
         <v>12</v>
       </c>
       <c r="C70">
-        <v>6.8</v>
+        <v>1.7</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E70" s="3">
         <v>1000</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
-      <c r="H70" s="4"/>
+      <c r="H70" s="6"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
       </c>
       <c r="C71">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E71" s="3">
         <v>1000</v>
       </c>
-      <c r="F71" s="3"/>
+      <c r="F71" s="3">
+        <v>0.9</v>
+      </c>
       <c r="G71" s="3"/>
       <c r="H71" s="6"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
       </c>
       <c r="C72">
-        <v>1.9</v>
+        <v>1.5</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E72" s="3">
         <v>1000</v>
       </c>
-      <c r="F72" s="3"/>
+      <c r="F72" s="3">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="G72" s="3"/>
       <c r="H72" s="6"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B73" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73">
-        <v>2.8</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C73"/>
       <c r="D73" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E73" s="3">
         <v>1000</v>
@@ -1977,16 +1934,11 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B74" t="s">
-        <v>12</v>
-      </c>
-      <c r="C74">
-        <v>2.1</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C74"/>
       <c r="D74" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E74" s="3">
         <v>1000</v>
@@ -1997,16 +1949,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
       </c>
       <c r="C75">
-        <v>3.4</v>
+        <v>1.9</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E75" s="3">
         <v>1000</v>
@@ -2017,126 +1969,124 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
       </c>
       <c r="C76">
-        <v>2.1</v>
+        <v>1</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E76" s="3">
         <v>1000</v>
       </c>
-      <c r="F76" s="3"/>
+      <c r="F76" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G76" s="3"/>
-      <c r="H76" s="6"/>
+      <c r="H76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B77" t="s">
         <v>12</v>
       </c>
       <c r="C77">
-        <v>4.5999999999999996</v>
+        <v>1</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E77" s="3">
         <v>1000</v>
       </c>
-      <c r="F77" s="3"/>
+      <c r="F77" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G77" s="3"/>
-      <c r="H77" s="4"/>
+      <c r="H77" s="6"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
         <v>12</v>
       </c>
       <c r="C78">
-        <v>5.3</v>
+        <v>1</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E78" s="3">
         <v>1000</v>
       </c>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="6"/>
+      <c r="F78" s="3">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B79" t="s">
-        <v>12</v>
-      </c>
-      <c r="C79">
-        <v>1.6</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C79"/>
       <c r="D79" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E79" s="3">
         <v>1000</v>
       </c>
       <c r="F79" s="3"/>
+      <c r="H79" s="3"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C80"/>
+        <v>20</v>
+      </c>
+      <c r="B80" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="D80" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E80" s="3">
         <v>1000</v>
       </c>
-      <c r="F80" s="3"/>
-      <c r="H80" s="3"/>
+      <c r="F80" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="G80" s="3"/>
+      <c r="H80" s="4"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B81" t="s">
-        <v>12</v>
-      </c>
-      <c r="C81">
-        <v>1.1000000000000001</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C81"/>
       <c r="D81" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E81" s="3">
         <v>1000</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
-      <c r="H81" s="4"/>
+      <c r="H81" s="5"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B82" t="s">
-        <v>12</v>
-      </c>
-      <c r="C82">
-        <v>1.5</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C82"/>
       <c r="D82" s="8" t="s">
         <v>13</v>
       </c>
@@ -2144,8 +2094,8 @@
         <v>1000</v>
       </c>
       <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="5"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
@@ -2159,41 +2109,29 @@
         <v>1000</v>
       </c>
       <c r="F83" s="3"/>
-      <c r="G83" s="6"/>
+      <c r="G83" s="3"/>
       <c r="H83" s="6"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B84" t="s">
-        <v>12</v>
-      </c>
-      <c r="C84">
-        <v>1.3</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C84"/>
       <c r="D84" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E84" s="3">
         <v>1000</v>
       </c>
-      <c r="F84" s="3">
-        <v>0.8</v>
-      </c>
+      <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="6"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B85" t="s">
-        <v>12</v>
-      </c>
-      <c r="C85">
-        <v>7.7</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C85"/>
       <c r="D85" s="8" t="s">
         <v>13</v>
       </c>
@@ -2206,14 +2144,9 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B86" t="s">
-        <v>12</v>
-      </c>
-      <c r="C86">
-        <v>2.9</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C86"/>
       <c r="D86" s="8" t="s">
         <v>13</v>
       </c>
@@ -2226,14 +2159,9 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B87" t="s">
-        <v>12</v>
-      </c>
-      <c r="C87">
-        <v>1.7</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C87"/>
       <c r="D87" s="8" t="s">
         <v>13</v>
       </c>
@@ -2242,33 +2170,35 @@
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
-      <c r="H87" s="6"/>
+      <c r="H87" s="4"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C88"/>
+        <v>26</v>
+      </c>
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88">
+        <v>1.4</v>
+      </c>
       <c r="D88" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E88" s="3">
         <v>1000</v>
       </c>
-      <c r="F88" s="3"/>
+      <c r="F88" s="3">
+        <v>1</v>
+      </c>
       <c r="G88" s="3"/>
-      <c r="H88" s="4"/>
+      <c r="H88" s="6"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B89" t="s">
-        <v>12</v>
-      </c>
-      <c r="C89">
-        <v>1.5</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C89"/>
       <c r="D89" s="8" t="s">
         <v>13</v>
       </c>
@@ -2281,9 +2211,14 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C90"/>
+        <v>17</v>
+      </c>
+      <c r="B90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90">
+        <v>1.4</v>
+      </c>
       <c r="D90" s="8" t="s">
         <v>13</v>
       </c>
@@ -2296,9 +2231,14 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C91"/>
+        <v>17</v>
+      </c>
+      <c r="B91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91">
+        <v>1.4</v>
+      </c>
       <c r="D91" s="8" t="s">
         <v>13</v>
       </c>
@@ -2311,31 +2251,29 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B92" t="s">
-        <v>12</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C92"/>
       <c r="D92" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E92" s="3">
         <v>1000</v>
       </c>
-      <c r="F92" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="6"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C93"/>
+        <v>22</v>
+      </c>
+      <c r="B93" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" s="10">
+        <v>3.2</v>
+      </c>
       <c r="D93" s="8" t="s">
         <v>13</v>
       </c>
@@ -2348,9 +2286,14 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C94" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="10">
+        <v>3.5</v>
+      </c>
       <c r="D94" s="8" t="s">
         <v>13</v>
       </c>
@@ -2359,17 +2302,17 @@
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
-      <c r="H94" s="6"/>
+      <c r="H94" s="4"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B95" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" t="s">
         <v>12</v>
       </c>
       <c r="C95" s="10">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>13</v>
@@ -2377,15 +2320,16 @@
       <c r="E95" s="3">
         <v>1000</v>
       </c>
-      <c r="F95" s="3"/>
+      <c r="F95" s="3">
+        <v>0.5</v>
+      </c>
       <c r="G95" s="3"/>
-      <c r="H95" s="4"/>
+      <c r="H95" s="6"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B96" s="3"/>
+        <v>17</v>
+      </c>
       <c r="C96" s="10"/>
       <c r="D96" s="8" t="s">
         <v>13</v>
@@ -2401,7 +2345,6 @@
       <c r="A97" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B97" s="3"/>
       <c r="C97" s="10"/>
       <c r="D97" s="8" t="s">
         <v>13</v>
@@ -2417,53 +2360,40 @@
       <c r="A98" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B98" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C98" s="10">
-        <v>1.7</v>
-      </c>
+      <c r="C98" s="10"/>
       <c r="D98" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E98" s="3">
         <v>1000</v>
       </c>
-      <c r="F98" s="3"/>
       <c r="G98" s="3"/>
       <c r="H98" s="6"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C99" s="10">
-        <v>1.1000000000000001</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C99" s="10"/>
       <c r="D99" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E99" s="3">
         <v>1000</v>
       </c>
-      <c r="F99">
-        <v>0.6</v>
-      </c>
+      <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="6"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B100" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B100" t="s">
         <v>12</v>
       </c>
-      <c r="C100" s="10">
-        <v>1</v>
+      <c r="C100" s="5">
+        <v>1.4</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>13</v>
@@ -2471,21 +2401,18 @@
       <c r="E100" s="3">
         <v>1000</v>
       </c>
-      <c r="F100" s="3">
-        <v>0.5</v>
-      </c>
       <c r="G100" s="3"/>
       <c r="H100" s="6"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B101" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B101" t="s">
         <v>12</v>
       </c>
       <c r="C101" s="5">
-        <v>1</v>
+        <v>3.6</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>13</v>
@@ -2493,21 +2420,12 @@
       <c r="E101" s="3">
         <v>1000</v>
       </c>
-      <c r="F101">
-        <v>0.5</v>
-      </c>
-      <c r="G101" s="3"/>
+      <c r="F101" s="3"/>
       <c r="H101" s="6"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C102" s="5">
-        <v>1.9</v>
+        <v>18</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>13</v>
@@ -2515,16 +2433,20 @@
       <c r="E102" s="3">
         <v>1000</v>
       </c>
-      <c r="F102" s="3">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
       <c r="H102" s="6"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B103" s="3"/>
+      <c r="B103" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103" s="5">
+        <v>2.9</v>
+      </c>
       <c r="D103" s="8" t="s">
         <v>13</v>
       </c>
@@ -2539,7 +2461,6 @@
       <c r="A104" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B104" s="3"/>
       <c r="D104" s="8" t="s">
         <v>13</v>
       </c>
@@ -2552,55 +2473,51 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B105" s="3"/>
+        <v>18</v>
+      </c>
       <c r="D105" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E105" s="3">
         <v>1000</v>
       </c>
       <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
       <c r="H105" s="6"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B106" s="3"/>
       <c r="D106" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E106" s="3">
         <v>1000</v>
       </c>
       <c r="F106" s="3"/>
-      <c r="H106" s="6"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="5"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B107" s="3"/>
+        <v>18</v>
+      </c>
       <c r="D107" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E107" s="3">
         <v>1000</v>
       </c>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
-      <c r="H107" s="5"/>
+      <c r="H107" s="6"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B108" s="3"/>
+        <v>21</v>
+      </c>
       <c r="D108" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E108" s="3">
         <v>1000</v>
@@ -2611,60 +2528,43 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B109" s="3"/>
+        <v>18</v>
+      </c>
       <c r="D109" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E109" s="3">
         <v>1000</v>
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
-      <c r="H109" s="6"/>
+      <c r="H109" s="4"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C110" s="5">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E110" s="3">
         <v>1000</v>
       </c>
-      <c r="F110" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="F110" s="3"/>
       <c r="G110" s="3"/>
-      <c r="H110" s="4"/>
+      <c r="H110" s="6"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C111" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E111" s="3">
         <v>1000</v>
       </c>
-      <c r="F111" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="F111" s="3"/>
       <c r="G111" s="3"/>
       <c r="H111" s="6"/>
     </row>
@@ -2672,9 +2572,8 @@
       <c r="A112" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B112" s="3"/>
       <c r="D112" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E112" s="3">
         <v>1000</v>
@@ -2685,41 +2584,36 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B113" s="3"/>
+        <v>18</v>
+      </c>
       <c r="D113" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E113" s="3">
         <v>1000</v>
       </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
-      <c r="H113" s="6"/>
+      <c r="H113" s="4"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B114" s="3"/>
+        <v>20</v>
+      </c>
       <c r="D114" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E114" s="3">
         <v>1000</v>
       </c>
-      <c r="F114" s="3"/>
-      <c r="G114" s="3"/>
-      <c r="H114" s="4"/>
+      <c r="H114" s="6"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B115" s="3"/>
+        <v>21</v>
+      </c>
       <c r="D115" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E115" s="3">
         <v>1000</v>
@@ -2728,24 +2622,22 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B116" s="3"/>
+        <v>18</v>
+      </c>
       <c r="D116" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E116" s="3">
         <v>1000</v>
       </c>
-      <c r="H116" s="6"/>
+      <c r="H116" s="4"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B117" s="3"/>
+        <v>20</v>
+      </c>
       <c r="D117" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E117" s="3">
         <v>1000</v>
@@ -2754,29 +2646,27 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B118" s="3"/>
+        <v>20</v>
+      </c>
       <c r="D118" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E118" s="3">
         <v>1000</v>
       </c>
-      <c r="H118" s="4"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B119" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B119" t="s">
         <v>12</v>
       </c>
       <c r="C119" s="5">
-        <v>1.2</v>
+        <v>2.7</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E119" s="3">
         <v>1000</v>
@@ -2784,66 +2674,47 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C120" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E120" s="3">
         <v>1000</v>
-      </c>
-      <c r="F120">
-        <v>0.5</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C121" s="5">
-        <v>1.1000000000000001</v>
+        <v>18</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E121" s="3">
         <v>1000</v>
       </c>
-      <c r="F121">
-        <v>1</v>
-      </c>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B122" s="3"/>
+        <v>18</v>
+      </c>
       <c r="D122" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E122" s="3">
         <v>1000</v>
       </c>
-      <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
-      <c r="H122" s="3"/>
+      <c r="H122" s="6"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B123" s="3"/>
+        <v>20</v>
+      </c>
       <c r="D123" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E123" s="3">
         <v>1000</v>
@@ -2852,68 +2723,58 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B124" s="3"/>
+        <v>17</v>
+      </c>
       <c r="D124" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E124" s="3">
         <v>1000</v>
       </c>
-      <c r="H124" s="6"/>
+      <c r="H124" s="9"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B125" s="3"/>
       <c r="D125" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E125" s="3">
         <v>1000</v>
       </c>
-      <c r="H125" s="9"/>
+      <c r="H125" s="6"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B126" s="3"/>
+        <v>20</v>
+      </c>
       <c r="D126" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E126" s="3">
         <v>1000</v>
       </c>
-      <c r="H126" s="6"/>
+      <c r="H126" s="4"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B127" s="3"/>
+        <v>18</v>
+      </c>
       <c r="D127" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E127" s="3">
         <v>1000</v>
       </c>
-      <c r="H127" s="4"/>
+      <c r="H127" s="6"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C128" s="5">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E128" s="3">
         <v>1000</v>
@@ -2924,14 +2785,9 @@
       <c r="A129" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B129" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C129" s="5">
-        <v>1.2</v>
-      </c>
+      <c r="B129" s="3"/>
       <c r="D129" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E129" s="3">
         <v>1000</v>
@@ -2940,129 +2796,235 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B130" s="3"/>
       <c r="D130" s="8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E130" s="3">
         <v>1000</v>
       </c>
-      <c r="H130" s="6"/>
+      <c r="H130" s="4"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="3"/>
+      <c r="A131" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="B131" s="3"/>
-      <c r="D131" s="8"/>
-      <c r="E131" s="3"/>
-      <c r="H131" s="4"/>
+      <c r="D131" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E131" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H131" s="6"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="3"/>
+      <c r="A132" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B132" s="3"/>
-      <c r="D132" s="8"/>
-      <c r="E132" s="3"/>
+      <c r="D132" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E132" s="3">
+        <v>1000</v>
+      </c>
       <c r="H132" s="6"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="3"/>
+      <c r="A133" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="B133" s="3"/>
-      <c r="D133" s="8"/>
-      <c r="E133" s="3"/>
+      <c r="D133" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E133" s="3">
+        <v>1000</v>
+      </c>
       <c r="H133" s="6"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A134" s="3"/>
+      <c r="A134" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="B134" s="3"/>
-      <c r="D134" s="8"/>
-      <c r="E134" s="3"/>
+      <c r="D134" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E134" s="3">
+        <v>1000</v>
+      </c>
       <c r="H134" s="6"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="3"/>
+      <c r="A135" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B135" s="3"/>
-      <c r="D135" s="8"/>
-      <c r="E135" s="3"/>
+      <c r="D135" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E135" s="3">
+        <v>1000</v>
+      </c>
       <c r="H135" s="6"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="3"/>
+      <c r="A136" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="B136" s="3"/>
-      <c r="D136" s="8"/>
-      <c r="E136" s="3"/>
+      <c r="D136" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E136" s="3">
+        <v>1000</v>
+      </c>
       <c r="H136" s="6"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="3"/>
+      <c r="A137" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B137" s="3"/>
-      <c r="D137" s="8"/>
-      <c r="E137" s="3"/>
+      <c r="D137" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E137" s="3">
+        <v>1000</v>
+      </c>
       <c r="H137" s="6"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="3"/>
+      <c r="A138" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="B138" s="3"/>
-      <c r="D138" s="8"/>
-      <c r="E138" s="3"/>
+      <c r="D138" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E138" s="3">
+        <v>1000</v>
+      </c>
       <c r="H138" s="6"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="3"/>
+      <c r="A139" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B139" s="3"/>
-      <c r="D139" s="8"/>
-      <c r="E139" s="3"/>
+      <c r="D139" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E139" s="3">
+        <v>1000</v>
+      </c>
       <c r="H139" s="6"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="3"/>
-      <c r="B140" s="3"/>
-      <c r="D140" s="8"/>
-      <c r="E140" s="3"/>
+      <c r="A140" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C140" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E140" s="3">
+        <v>1000</v>
+      </c>
       <c r="H140" s="6"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="3"/>
+      <c r="A141" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="B141" s="3"/>
-      <c r="D141" s="8"/>
-      <c r="E141" s="3"/>
+      <c r="D141" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E141" s="3">
+        <v>1000</v>
+      </c>
       <c r="H141" s="6"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="3"/>
-      <c r="B142" s="3"/>
-      <c r="D142" s="8"/>
-      <c r="E142" s="3"/>
+      <c r="A142" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C142" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E142" s="3">
+        <v>1000</v>
+      </c>
       <c r="H142" s="6"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A143" s="3"/>
+      <c r="A143" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B143" s="3"/>
-      <c r="D143" s="8"/>
-      <c r="E143" s="3"/>
-      <c r="H143" s="6"/>
+      <c r="D143" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E143" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F143" s="3"/>
+      <c r="G143" s="3"/>
+      <c r="H143" s="4"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="3"/>
+      <c r="A144" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="B144" s="3"/>
-      <c r="D144" s="8"/>
-      <c r="E144" s="3"/>
-      <c r="F144" s="3"/>
-      <c r="G144" s="3"/>
-      <c r="H144" s="4"/>
+      <c r="D144" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E144" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H144" s="6"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A145" s="3"/>
+      <c r="A145" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="B145" s="3"/>
-      <c r="D145" s="8"/>
-      <c r="E145" s="3"/>
+      <c r="D145" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E145" s="3">
+        <v>1000</v>
+      </c>
       <c r="H145" s="6"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A146" s="3"/>
+      <c r="A146" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="B146" s="3"/>
-      <c r="D146" s="8"/>
-      <c r="E146" s="3"/>
+      <c r="D146" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E146" s="3">
+        <v>1000</v>
+      </c>
       <c r="H146" s="6"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -3070,14 +3032,14 @@
       <c r="B147" s="3"/>
       <c r="D147" s="8"/>
       <c r="E147" s="3"/>
-      <c r="H147" s="6"/>
+      <c r="H147" s="4"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="D148" s="8"/>
       <c r="E148" s="3"/>
-      <c r="H148" s="4"/>
+      <c r="H148" s="6"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="3"/>
@@ -3129,16 +3091,17 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="3"/>
+      <c r="B156" s="3"/>
       <c r="D156" s="8"/>
       <c r="E156" s="3"/>
-      <c r="H156" s="6"/>
+      <c r="H156" s="4"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="D157" s="8"/>
       <c r="E157" s="3"/>
-      <c r="H157" s="4"/>
+      <c r="H157" s="6"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
@@ -3152,6 +3115,7 @@
       <c r="B159" s="3"/>
       <c r="D159" s="8"/>
       <c r="E159" s="3"/>
+      <c r="G159" s="3"/>
       <c r="H159" s="6"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -3159,7 +3123,6 @@
       <c r="B160" s="3"/>
       <c r="D160" s="8"/>
       <c r="E160" s="3"/>
-      <c r="G160" s="3"/>
       <c r="H160" s="6"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -3178,7 +3141,6 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="3"/>
-      <c r="B163" s="3"/>
       <c r="D163" s="8"/>
       <c r="E163" s="3"/>
       <c r="H163" s="6"/>
@@ -3191,6 +3153,7 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
+      <c r="B165" s="3"/>
       <c r="D165" s="8"/>
       <c r="E165" s="3"/>
       <c r="H165" s="6"/>
@@ -3204,7 +3167,6 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="3"/>
-      <c r="B167" s="3"/>
       <c r="D167" s="8"/>
       <c r="E167" s="3"/>
       <c r="H167" s="6"/>
@@ -3231,13 +3193,13 @@
       <c r="A171" s="3"/>
       <c r="D171" s="8"/>
       <c r="E171" s="3"/>
-      <c r="H171" s="6"/>
+      <c r="H171" s="3"/>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="3"/>
       <c r="D172" s="8"/>
       <c r="E172" s="3"/>
-      <c r="H172" s="3"/>
+      <c r="H172" s="6"/>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="3"/>
@@ -3249,13 +3211,13 @@
       <c r="A174" s="3"/>
       <c r="D174" s="8"/>
       <c r="E174" s="3"/>
-      <c r="H174" s="6"/>
+      <c r="H174" s="3"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="3"/>
       <c r="D175" s="8"/>
       <c r="E175" s="3"/>
-      <c r="H175" s="3"/>
+      <c r="H175" s="6"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="3"/>
@@ -3279,18 +3241,18 @@
       <c r="A179" s="3"/>
       <c r="D179" s="8"/>
       <c r="E179" s="3"/>
-      <c r="H179" s="6"/>
+      <c r="H179" s="4"/>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="3"/>
       <c r="D180" s="8"/>
       <c r="E180" s="3"/>
-      <c r="H180" s="4"/>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="3"/>
       <c r="D181" s="8"/>
       <c r="E181" s="3"/>
+      <c r="H181" s="6"/>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="3"/>
@@ -3314,12 +3276,12 @@
       <c r="A185" s="3"/>
       <c r="D185" s="8"/>
       <c r="E185" s="3"/>
-      <c r="H185" s="6"/>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="3"/>
       <c r="D186" s="8"/>
       <c r="E186" s="3"/>
+      <c r="H186" s="4"/>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="3"/>
@@ -3331,7 +3293,7 @@
       <c r="A188" s="3"/>
       <c r="D188" s="8"/>
       <c r="E188" s="3"/>
-      <c r="H188" s="4"/>
+      <c r="H188" s="6"/>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="3"/>
@@ -3379,7 +3341,7 @@
       <c r="A196" s="3"/>
       <c r="D196" s="8"/>
       <c r="E196" s="3"/>
-      <c r="H196" s="6"/>
+      <c r="H196" s="4"/>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="3"/>
@@ -3391,7 +3353,7 @@
       <c r="A198" s="3"/>
       <c r="D198" s="8"/>
       <c r="E198" s="3"/>
-      <c r="H198" s="4"/>
+      <c r="H198" s="6"/>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="3"/>
@@ -3427,7 +3389,8 @@
       <c r="A204" s="3"/>
       <c r="D204" s="8"/>
       <c r="E204" s="3"/>
-      <c r="H204" s="6"/>
+      <c r="G204" s="6"/>
+      <c r="H204" s="4"/>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="3"/>
@@ -3440,55 +3403,54 @@
       <c r="A206" s="3"/>
       <c r="D206" s="8"/>
       <c r="E206" s="3"/>
-      <c r="G206" s="6"/>
-      <c r="H206" s="4"/>
+      <c r="H206" s="6"/>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="3"/>
       <c r="D207" s="8"/>
       <c r="E207" s="3"/>
-      <c r="H207" s="6"/>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="3"/>
       <c r="D208" s="8"/>
       <c r="E208" s="3"/>
+      <c r="H208" s="6"/>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" s="3"/>
       <c r="D209" s="8"/>
       <c r="E209" s="3"/>
-      <c r="H209" s="6"/>
+      <c r="H209" s="4"/>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" s="3"/>
       <c r="D210" s="8"/>
       <c r="E210" s="3"/>
-      <c r="H210" s="4"/>
+      <c r="H210" s="6"/>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" s="3"/>
       <c r="D211" s="8"/>
       <c r="E211" s="3"/>
-      <c r="H211" s="6"/>
+      <c r="H211" s="4"/>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" s="3"/>
       <c r="D212" s="8"/>
       <c r="E212" s="3"/>
-      <c r="H212" s="4"/>
+      <c r="H212" s="6"/>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" s="3"/>
       <c r="D213" s="8"/>
       <c r="E213" s="3"/>
-      <c r="H213" s="6"/>
+      <c r="H213" s="4"/>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" s="3"/>
       <c r="D214" s="8"/>
       <c r="E214" s="3"/>
-      <c r="H214" s="4"/>
+      <c r="H214" s="6"/>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" s="3"/>
@@ -3524,13 +3486,13 @@
       <c r="A220" s="3"/>
       <c r="D220" s="8"/>
       <c r="E220" s="3"/>
-      <c r="H220" s="6"/>
+      <c r="H220" s="4"/>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="3"/>
       <c r="D221" s="8"/>
       <c r="E221" s="3"/>
-      <c r="H221" s="4"/>
+      <c r="H221" s="6"/>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" s="3"/>
@@ -3542,7 +3504,6 @@
       <c r="A223" s="3"/>
       <c r="D223" s="8"/>
       <c r="E223" s="3"/>
-      <c r="H223" s="6"/>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" s="3"/>
@@ -3563,36 +3524,36 @@
       <c r="A227" s="3"/>
       <c r="D227" s="8"/>
       <c r="E227" s="3"/>
+      <c r="H227" s="6"/>
     </row>
     <row r="228" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A228" s="3"/>
       <c r="D228" s="8"/>
       <c r="E228" s="3"/>
-      <c r="H228" s="6"/>
     </row>
     <row r="229" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A229" s="3"/>
       <c r="D229" s="8"/>
       <c r="E229" s="3"/>
+      <c r="H229" s="6"/>
+      <c r="XFD229" s="6"/>
     </row>
     <row r="230" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A230" s="3"/>
       <c r="D230" s="8"/>
       <c r="E230" s="3"/>
-      <c r="H230" s="6"/>
-      <c r="XFD230" s="6"/>
+      <c r="H230" s="4"/>
     </row>
     <row r="231" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A231" s="3"/>
       <c r="D231" s="8"/>
       <c r="E231" s="3"/>
-      <c r="H231" s="4"/>
+      <c r="H231" s="6"/>
     </row>
     <row r="232" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A232" s="3"/>
       <c r="D232" s="8"/>
       <c r="E232" s="3"/>
-      <c r="H232" s="6"/>
     </row>
     <row r="233" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A233" s="3"/>
@@ -3603,12 +3564,12 @@
       <c r="A234" s="3"/>
       <c r="D234" s="8"/>
       <c r="E234" s="3"/>
+      <c r="H234" s="4"/>
     </row>
     <row r="235" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A235" s="3"/>
       <c r="D235" s="8"/>
       <c r="E235" s="3"/>
-      <c r="H235" s="4"/>
     </row>
     <row r="236" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A236" s="3"/>
@@ -3624,6 +3585,7 @@
       <c r="A238" s="3"/>
       <c r="D238" s="8"/>
       <c r="E238" s="3"/>
+      <c r="H238" s="6"/>
     </row>
     <row r="239" spans="1:8 16384:16384" x14ac:dyDescent="0.2">
       <c r="A239" s="3"/>
@@ -3635,19 +3597,18 @@
       <c r="A240" s="3"/>
       <c r="D240" s="8"/>
       <c r="E240" s="3"/>
-      <c r="H240" s="6"/>
+      <c r="H240" s="4"/>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" s="3"/>
       <c r="D241" s="8"/>
       <c r="E241" s="3"/>
-      <c r="H241" s="4"/>
+      <c r="H241" s="6"/>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" s="3"/>
       <c r="D242" s="8"/>
       <c r="E242" s="3"/>
-      <c r="H242" s="6"/>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" s="3"/>
@@ -3658,12 +3619,12 @@
       <c r="A244" s="3"/>
       <c r="D244" s="8"/>
       <c r="E244" s="3"/>
+      <c r="H244" s="6"/>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" s="3"/>
       <c r="D245" s="8"/>
       <c r="E245" s="3"/>
-      <c r="H245" s="6"/>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" s="3"/>
@@ -3674,12 +3635,12 @@
       <c r="A247" s="3"/>
       <c r="D247" s="8"/>
       <c r="E247" s="3"/>
+      <c r="H247" s="4"/>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" s="3"/>
       <c r="D248" s="8"/>
       <c r="E248" s="3"/>
-      <c r="H248" s="4"/>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" s="3"/>
@@ -3695,12 +3656,12 @@
       <c r="A251" s="3"/>
       <c r="D251" s="8"/>
       <c r="E251" s="3"/>
+      <c r="H251" s="4"/>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" s="3"/>
       <c r="D252" s="8"/>
       <c r="E252" s="3"/>
-      <c r="H252" s="4"/>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" s="3"/>
@@ -3711,6 +3672,7 @@
       <c r="A254" s="3"/>
       <c r="D254" s="8"/>
       <c r="E254" s="3"/>
+      <c r="H254" s="4"/>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" s="3"/>
@@ -3722,24 +3684,23 @@
       <c r="A256" s="3"/>
       <c r="D256" s="8"/>
       <c r="E256" s="3"/>
-      <c r="H256" s="4"/>
+      <c r="H256" s="6"/>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" s="3"/>
       <c r="D257" s="8"/>
       <c r="E257" s="3"/>
-      <c r="H257" s="6"/>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" s="3"/>
       <c r="D258" s="8"/>
       <c r="E258" s="3"/>
+      <c r="H258" s="4"/>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" s="3"/>
       <c r="D259" s="8"/>
       <c r="E259" s="3"/>
-      <c r="H259" s="4"/>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" s="3"/>
@@ -3760,6 +3721,7 @@
       <c r="A263" s="3"/>
       <c r="D263" s="8"/>
       <c r="E263" s="3"/>
+      <c r="H263" s="6"/>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" s="3"/>
@@ -3783,35 +3745,35 @@
       <c r="A267" s="3"/>
       <c r="D267" s="8"/>
       <c r="E267" s="3"/>
-      <c r="H267" s="6"/>
+      <c r="H267" s="3"/>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" s="3"/>
       <c r="D268" s="8"/>
       <c r="E268" s="3"/>
-      <c r="H268" s="3"/>
+      <c r="H268" s="4"/>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" s="3"/>
       <c r="D269" s="8"/>
       <c r="E269" s="3"/>
-      <c r="H269" s="4"/>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" s="3"/>
       <c r="D270" s="8"/>
       <c r="E270" s="3"/>
+      <c r="H270" s="3"/>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" s="3"/>
       <c r="D271" s="8"/>
       <c r="E271" s="3"/>
-      <c r="H271" s="3"/>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" s="3"/>
       <c r="D272" s="8"/>
       <c r="E272" s="3"/>
+      <c r="H272" s="4"/>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" s="3"/>
@@ -3829,7 +3791,6 @@
       <c r="A275" s="3"/>
       <c r="D275" s="8"/>
       <c r="E275" s="3"/>
-      <c r="H275" s="4"/>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" s="3"/>
@@ -3845,12 +3806,12 @@
       <c r="A278" s="3"/>
       <c r="D278" s="8"/>
       <c r="E278" s="3"/>
+      <c r="H278" s="6"/>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" s="3"/>
       <c r="D279" s="8"/>
       <c r="E279" s="3"/>
-      <c r="H279" s="6"/>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A280" s="3"/>
@@ -3861,18 +3822,18 @@
       <c r="A281" s="3"/>
       <c r="D281" s="8"/>
       <c r="E281" s="3"/>
+      <c r="H281" s="4"/>
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A282" s="3"/>
       <c r="D282" s="8"/>
       <c r="E282" s="3"/>
-      <c r="H282" s="4"/>
+      <c r="H282" s="6"/>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A283" s="3"/>
       <c r="D283" s="8"/>
       <c r="E283" s="3"/>
-      <c r="H283" s="6"/>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A284" s="3"/>
@@ -3883,12 +3844,13 @@
       <c r="A285" s="3"/>
       <c r="D285" s="8"/>
       <c r="E285" s="3"/>
+      <c r="H285" s="4"/>
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A286" s="3"/>
       <c r="D286" s="8"/>
       <c r="E286" s="3"/>
-      <c r="H286" s="4"/>
+      <c r="H286" s="6"/>
     </row>
     <row r="287" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A287" s="3"/>
@@ -3900,7 +3862,7 @@
       <c r="A288" s="3"/>
       <c r="D288" s="8"/>
       <c r="E288" s="3"/>
-      <c r="H288" s="6"/>
+      <c r="H288" s="4"/>
     </row>
     <row r="289" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A289" s="3"/>
@@ -3909,10 +3871,9 @@
       <c r="H289" s="4"/>
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A290" s="3"/>
+      <c r="A290" s="4"/>
       <c r="D290" s="8"/>
       <c r="E290" s="3"/>
-      <c r="H290" s="4"/>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A291" s="4"/>
@@ -3923,12 +3884,12 @@
       <c r="A292" s="4"/>
       <c r="D292" s="8"/>
       <c r="E292" s="3"/>
+      <c r="H292" s="6"/>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A293" s="4"/>
       <c r="D293" s="8"/>
       <c r="E293" s="3"/>
-      <c r="H293" s="6"/>
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A294" s="4"/>
@@ -3939,12 +3900,12 @@
       <c r="A295" s="4"/>
       <c r="D295" s="8"/>
       <c r="E295" s="3"/>
+      <c r="H295" s="6"/>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A296" s="4"/>
       <c r="D296" s="8"/>
       <c r="E296" s="3"/>
-      <c r="H296" s="6"/>
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A297" s="4"/>
@@ -3955,23 +3916,23 @@
       <c r="A298" s="4"/>
       <c r="D298" s="8"/>
       <c r="E298" s="3"/>
+      <c r="H298" s="4"/>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A299" s="4"/>
       <c r="D299" s="8"/>
       <c r="E299" s="3"/>
-      <c r="H299" s="4"/>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A300" s="4"/>
       <c r="D300" s="8"/>
       <c r="E300" s="3"/>
+      <c r="H300" s="6"/>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A301" s="4"/>
       <c r="D301" s="8"/>
       <c r="E301" s="3"/>
-      <c r="H301" s="6"/>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A302" s="4"/>
@@ -4022,12 +3983,12 @@
       <c r="A311" s="4"/>
       <c r="D311" s="8"/>
       <c r="E311" s="3"/>
+      <c r="H311" s="3"/>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A312" s="4"/>
       <c r="D312" s="8"/>
       <c r="E312" s="3"/>
-      <c r="H312" s="3"/>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A313" s="4"/>
@@ -4073,23 +4034,23 @@
       <c r="A321" s="4"/>
       <c r="D321" s="8"/>
       <c r="E321" s="3"/>
+      <c r="H321" s="4"/>
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A322" s="4"/>
       <c r="D322" s="8"/>
       <c r="E322" s="3"/>
-      <c r="H322" s="4"/>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A323" s="4"/>
       <c r="D323" s="8"/>
       <c r="E323" s="3"/>
+      <c r="G323" s="4"/>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A324" s="4"/>
       <c r="D324" s="8"/>
       <c r="E324" s="3"/>
-      <c r="G324" s="4"/>
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A325" s="4"/>
@@ -4175,12 +4136,12 @@
       <c r="A341" s="4"/>
       <c r="D341" s="8"/>
       <c r="E341" s="3"/>
+      <c r="H341" s="6"/>
     </row>
     <row r="342" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A342" s="4"/>
       <c r="D342" s="8"/>
       <c r="E342" s="3"/>
-      <c r="H342" s="6"/>
     </row>
     <row r="343" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A343" s="4"/>
@@ -4396,12 +4357,12 @@
       <c r="A385" s="4"/>
       <c r="D385" s="8"/>
       <c r="E385" s="3"/>
+      <c r="H385" s="3"/>
     </row>
     <row r="386" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A386" s="4"/>
       <c r="D386" s="8"/>
       <c r="E386" s="3"/>
-      <c r="H386" s="3"/>
     </row>
     <row r="387" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A387" s="4"/>
@@ -4432,12 +4393,12 @@
       <c r="A392" s="4"/>
       <c r="D392" s="8"/>
       <c r="E392" s="3"/>
+      <c r="H392" s="4"/>
     </row>
     <row r="393" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A393" s="4"/>
       <c r="D393" s="8"/>
       <c r="E393" s="3"/>
-      <c r="H393" s="4"/>
     </row>
     <row r="394" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A394" s="4"/>
@@ -4448,12 +4409,12 @@
       <c r="A395" s="4"/>
       <c r="D395" s="8"/>
       <c r="E395" s="3"/>
+      <c r="H395" s="4"/>
     </row>
     <row r="396" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A396" s="4"/>
       <c r="D396" s="8"/>
       <c r="E396" s="3"/>
-      <c r="H396" s="4"/>
     </row>
     <row r="397" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A397" s="4"/>
@@ -4469,12 +4430,12 @@
       <c r="A399" s="4"/>
       <c r="D399" s="8"/>
       <c r="E399" s="3"/>
+      <c r="H399" s="4"/>
     </row>
     <row r="400" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A400" s="4"/>
       <c r="D400" s="8"/>
       <c r="E400" s="3"/>
-      <c r="H400" s="4"/>
     </row>
     <row r="401" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A401" s="4"/>
@@ -4515,12 +4476,12 @@
       <c r="A408" s="4"/>
       <c r="D408" s="8"/>
       <c r="E408" s="3"/>
+      <c r="H408" s="4"/>
     </row>
     <row r="409" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A409" s="4"/>
       <c r="D409" s="8"/>
       <c r="E409" s="3"/>
-      <c r="H409" s="4"/>
     </row>
     <row r="410" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A410" s="4"/>
@@ -4561,12 +4522,12 @@
       <c r="A417" s="4"/>
       <c r="D417" s="8"/>
       <c r="E417" s="3"/>
+      <c r="H417" s="4"/>
     </row>
     <row r="418" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A418" s="4"/>
       <c r="D418" s="8"/>
       <c r="E418" s="3"/>
-      <c r="H418" s="4"/>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A419" s="4"/>
@@ -4597,12 +4558,12 @@
       <c r="A424" s="4"/>
       <c r="D424" s="8"/>
       <c r="E424" s="3"/>
+      <c r="H424" s="4"/>
     </row>
     <row r="425" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A425" s="4"/>
       <c r="D425" s="8"/>
       <c r="E425" s="3"/>
-      <c r="H425" s="4"/>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A426" s="4"/>
@@ -4658,6 +4619,7 @@
       <c r="A436" s="4"/>
       <c r="D436" s="8"/>
       <c r="E436" s="3"/>
+      <c r="H436" s="4"/>
     </row>
     <row r="437" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A437" s="4"/>
@@ -4669,7 +4631,6 @@
       <c r="A438" s="4"/>
       <c r="D438" s="8"/>
       <c r="E438" s="3"/>
-      <c r="H438" s="4"/>
     </row>
     <row r="439" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A439" s="4"/>
@@ -4680,12 +4641,12 @@
       <c r="A440" s="4"/>
       <c r="D440" s="8"/>
       <c r="E440" s="3"/>
+      <c r="H440" s="4"/>
     </row>
     <row r="441" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A441" s="4"/>
       <c r="D441" s="8"/>
       <c r="E441" s="3"/>
-      <c r="H441" s="4"/>
     </row>
     <row r="442" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A442" s="4"/>
@@ -4722,92 +4683,92 @@
       <c r="D448" s="8"/>
       <c r="E448" s="3"/>
     </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A449" s="4"/>
       <c r="D449" s="8"/>
       <c r="E449" s="3"/>
     </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A450" s="4"/>
       <c r="D450" s="8"/>
       <c r="E450" s="3"/>
-    </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F450" s="3"/>
+    </row>
+    <row r="451" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A451" s="4"/>
       <c r="D451" s="8"/>
       <c r="E451" s="3"/>
-      <c r="F451" s="3"/>
-    </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="452" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A452" s="4"/>
       <c r="D452" s="8"/>
       <c r="E452" s="3"/>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A453" s="4"/>
       <c r="D453" s="8"/>
       <c r="E453" s="3"/>
     </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A454" s="4"/>
       <c r="D454" s="8"/>
       <c r="E454" s="3"/>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A455" s="4"/>
       <c r="D455" s="8"/>
       <c r="E455" s="3"/>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A456" s="4"/>
       <c r="D456" s="8"/>
       <c r="E456" s="3"/>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A457" s="4"/>
       <c r="D457" s="8"/>
       <c r="E457" s="3"/>
     </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A458" s="4"/>
       <c r="D458" s="8"/>
       <c r="E458" s="3"/>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A459" s="4"/>
       <c r="D459" s="8"/>
       <c r="E459" s="3"/>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A460" s="4"/>
       <c r="D460" s="8"/>
       <c r="E460" s="3"/>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A461" s="4"/>
       <c r="D461" s="8"/>
       <c r="E461" s="3"/>
     </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A462" s="4"/>
       <c r="D462" s="8"/>
       <c r="E462" s="3"/>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A463" s="4"/>
       <c r="D463" s="8"/>
       <c r="E463" s="3"/>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A464" s="4"/>
       <c r="D464" s="8"/>
       <c r="E464" s="3"/>
+      <c r="H464" s="3"/>
     </row>
     <row r="465" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A465" s="4"/>
       <c r="D465" s="8"/>
       <c r="E465" s="3"/>
-      <c r="H465" s="3"/>
     </row>
     <row r="466" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A466" s="4"/>
@@ -4838,12 +4799,12 @@
       <c r="A471" s="4"/>
       <c r="D471" s="8"/>
       <c r="E471" s="3"/>
+      <c r="H471" s="3"/>
     </row>
     <row r="472" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A472" s="4"/>
       <c r="D472" s="8"/>
       <c r="E472" s="3"/>
-      <c r="H472" s="3"/>
     </row>
     <row r="473" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A473" s="4"/>
@@ -4909,12 +4870,12 @@
       <c r="A485" s="4"/>
       <c r="D485" s="8"/>
       <c r="E485" s="3"/>
+      <c r="H485" s="4"/>
     </row>
     <row r="486" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A486" s="4"/>
       <c r="D486" s="8"/>
       <c r="E486" s="3"/>
-      <c r="H486" s="4"/>
     </row>
     <row r="487" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A487" s="4"/>
@@ -5095,12 +5056,12 @@
       <c r="A522" s="4"/>
       <c r="D522" s="8"/>
       <c r="E522" s="3"/>
+      <c r="H522" s="4"/>
     </row>
     <row r="523" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A523" s="4"/>
       <c r="D523" s="8"/>
       <c r="E523" s="3"/>
-      <c r="H523" s="4"/>
     </row>
     <row r="524" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A524" s="4"/>
@@ -5166,12 +5127,12 @@
       <c r="A536" s="4"/>
       <c r="D536" s="8"/>
       <c r="E536" s="3"/>
+      <c r="H536" s="4"/>
     </row>
     <row r="537" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A537" s="4"/>
       <c r="D537" s="8"/>
       <c r="E537" s="3"/>
-      <c r="H537" s="4"/>
     </row>
     <row r="538" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A538" s="4"/>
@@ -5567,6 +5528,7 @@
       <c r="A616" s="4"/>
       <c r="D616" s="8"/>
       <c r="E616" s="3"/>
+      <c r="H616" s="4"/>
     </row>
     <row r="617" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A617" s="4"/>
@@ -5578,7 +5540,6 @@
       <c r="A618" s="4"/>
       <c r="D618" s="8"/>
       <c r="E618" s="3"/>
-      <c r="H618" s="4"/>
     </row>
     <row r="619" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A619" s="4"/>
@@ -5587,7 +5548,7 @@
     </row>
     <row r="620" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A620" s="4"/>
-      <c r="D620" s="8"/>
+      <c r="D620" s="3"/>
       <c r="E620" s="3"/>
     </row>
     <row r="621" spans="1:8" x14ac:dyDescent="0.2">
@@ -8121,7 +8082,6 @@
       <c r="E1126" s="3"/>
     </row>
     <row r="1127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1127" s="4"/>
       <c r="D1127" s="3"/>
       <c r="E1127" s="3"/>
     </row>
@@ -8175,13 +8135,9 @@
     </row>
     <row r="1140" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D1140" s="3"/>
-      <c r="E1140" s="3"/>
-    </row>
-    <row r="1141" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D1141" s="3"/>
-    </row>
-    <row r="1048574" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H1048574" s="6"/>
+    </row>
+    <row r="1048573" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H1048573" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>